<commit_message>
cahier de recette maj
</commit_message>
<xml_diff>
--- a/documentation/FinalGanttJEAN.xlsx
+++ b/documentation/FinalGanttJEAN.xlsx
@@ -1129,8 +1129,8 @@
   </sheetPr>
   <dimension ref="B1:HC30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2022,7 +2022,7 @@
       <c r="HB5" s="1"/>
       <c r="HC5" s="1"/>
     </row>
-    <row r="6" spans="2:211" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:211" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18"/>
       <c r="F6" s="24" t="s">
         <v>15</v>
@@ -2183,7 +2183,7 @@
       <c r="HB6" s="1"/>
       <c r="HC6" s="1"/>
     </row>
-    <row r="7" spans="2:211" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:211" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18"/>
       <c r="F7" s="24" t="s">
         <v>16</v>
@@ -2344,7 +2344,7 @@
       <c r="HB7" s="1"/>
       <c r="HC7" s="1"/>
     </row>
-    <row r="8" spans="2:211" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:211" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="18"/>
       <c r="F8" s="24" t="s">
         <v>17</v>
@@ -2505,7 +2505,7 @@
       <c r="HB8" s="1"/>
       <c r="HC8" s="1"/>
     </row>
-    <row r="9" spans="2:211" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:211" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="18"/>
       <c r="F9" s="24" t="s">
         <v>21</v>
@@ -2666,7 +2666,7 @@
       <c r="HB9" s="1"/>
       <c r="HC9" s="1"/>
     </row>
-    <row r="10" spans="2:211" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:211" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="18"/>
       <c r="F10" s="24" t="s">
         <v>18</v>
@@ -2681,7 +2681,7 @@
         <v>120</v>
       </c>
       <c r="J10" s="25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K10" s="23">
         <v>1</v>
@@ -2827,7 +2827,7 @@
       <c r="HB10" s="1"/>
       <c r="HC10" s="1"/>
     </row>
-    <row r="11" spans="2:211" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:211" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="18"/>
       <c r="F11" s="24" t="s">
         <v>22</v>
@@ -2988,7 +2988,7 @@
       <c r="HB11" s="1"/>
       <c r="HC11" s="1"/>
     </row>
-    <row r="12" spans="2:211" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:211" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="18"/>
       <c r="F12" s="24" t="s">
         <v>19</v>
@@ -3149,7 +3149,7 @@
       <c r="HB12" s="1"/>
       <c r="HC12" s="1"/>
     </row>
-    <row r="13" spans="2:211" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:211" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="18"/>
       <c r="F13" s="24" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
excel maj cases figées
</commit_message>
<xml_diff>
--- a/documentation/FinalGanttJEAN.xlsx
+++ b/documentation/FinalGanttJEAN.xlsx
@@ -1129,14 +1129,17 @@
   </sheetPr>
   <dimension ref="B1:HC30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="2.625" customWidth="1"/>
-    <col min="6" max="6" width="15.625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="38.375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="16.625" style="1" customWidth="1"/>
     <col min="11" max="11" width="25.375" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3.25" style="1"/>

</xml_diff>